<commit_message>
First Working Module without any styling
</commit_message>
<xml_diff>
--- a/src/utils/friends_data.xlsx
+++ b/src/utils/friends_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="states" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="73">
   <si>
     <t>Node</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>Connection</t>
-  </si>
-  <si>
-    <t>null</t>
   </si>
   <si>
     <t>BENGALURU</t>
@@ -566,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,16 +585,16 @@
         <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>42</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -607,17 +604,17 @@
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>28</v>
+      <c r="C2">
+        <v>503</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -627,17 +624,17 @@
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>28</v>
+      <c r="C3">
+        <v>1873</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -647,17 +644,17 @@
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
-        <v>28</v>
+      <c r="C4">
+        <v>8068</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -667,17 +664,17 @@
       <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
-        <v>28</v>
+      <c r="C5">
+        <v>2185</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -687,17 +684,17 @@
       <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
-        <v>28</v>
+      <c r="C6">
+        <v>469</v>
       </c>
       <c r="D6" t="s">
         <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -707,17 +704,17 @@
       <c r="B7" t="s">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
-        <v>28</v>
+      <c r="C7">
+        <v>2918</v>
       </c>
       <c r="D7" t="s">
         <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -729,7 +726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -751,16 +748,16 @@
         <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>42</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -771,16 +768,16 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -791,16 +788,16 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -811,16 +808,16 @@
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -831,16 +828,16 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -851,16 +848,16 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -871,16 +868,16 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -891,16 +888,16 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -911,16 +908,16 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -931,16 +928,16 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -951,16 +948,16 @@
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -971,16 +968,16 @@
         <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -991,16 +988,16 @@
         <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1011,16 +1008,16 @@
         <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1031,16 +1028,16 @@
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
         <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1051,16 +1048,16 @@
         <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
         <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1071,16 +1068,16 @@
         <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
         <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1091,16 +1088,16 @@
         <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s">
         <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1111,16 +1108,16 @@
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D19" t="s">
         <v>23</v>
       </c>
       <c r="E19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1137,10 +1134,10 @@
         <v>24</v>
       </c>
       <c r="E20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1151,16 +1148,16 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D21" t="s">
         <v>26</v>
       </c>
       <c r="E21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>